<commit_message>
!3746 doc(#I69VD0): update fileviewer demos * reformat code * update fileviewer demos
</commit_message>
<xml_diff>
--- a/src/BootstrapBlazor.Server/wwwroot/samples/sample3.xlsx
+++ b/src/BootstrapBlazor.Server/wwwroot/samples/sample3.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{695153B2-8866-4884-903A-2AADF4AD2AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FE8EEE-B479-45B4-86FD-FB6999784806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15034" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="每周家务安排表" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="First_Day">每周家务安排表!$C$3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,9 +21,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>任务</t>
   </si>
@@ -103,6 +101,34 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>2023-01-01</t>
+    <phoneticPr fontId="25" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023-01-02</t>
+    <phoneticPr fontId="25" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023-01-03</t>
+    <phoneticPr fontId="25" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023-01-04</t>
+    <phoneticPr fontId="25" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023-01-05</t>
+    <phoneticPr fontId="25" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023-01-06</t>
+    <phoneticPr fontId="25" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023-01-07</t>
+    <phoneticPr fontId="25" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -870,28 +896,28 @@
     <xf numFmtId="178" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="22" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="22" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2711,31 +2737,33 @@
   </sheetPr>
   <dimension ref="B1:Q21"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.796875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.19921875" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.796875" style="14" customWidth="1"/>
-    <col min="4" max="4" width="7.796875" style="18" customWidth="1"/>
-    <col min="5" max="5" width="7.796875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="7.796875" style="19" customWidth="1"/>
-    <col min="7" max="7" width="7.796875" style="14" customWidth="1"/>
-    <col min="8" max="8" width="7.796875" style="19" customWidth="1"/>
-    <col min="9" max="9" width="7.796875" style="14" customWidth="1"/>
-    <col min="10" max="10" width="7.796875" style="19" customWidth="1"/>
-    <col min="11" max="11" width="7.796875" style="14" customWidth="1"/>
-    <col min="12" max="12" width="7.796875" style="19" customWidth="1"/>
-    <col min="13" max="13" width="7.796875" style="14" customWidth="1"/>
-    <col min="14" max="14" width="7.796875" style="19" customWidth="1"/>
-    <col min="15" max="15" width="7.796875" style="14" customWidth="1"/>
-    <col min="16" max="16" width="7.796875" style="19" customWidth="1"/>
-    <col min="17" max="17" width="1.796875" style="14" customWidth="1"/>
-    <col min="18" max="16384" width="9.1328125" style="14"/>
+    <col min="1" max="1" width="1.77734375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="7.77734375" style="18" customWidth="1"/>
+    <col min="5" max="5" width="7.77734375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" style="19" customWidth="1"/>
+    <col min="7" max="7" width="7.77734375" style="14" customWidth="1"/>
+    <col min="8" max="8" width="7.77734375" style="19" customWidth="1"/>
+    <col min="9" max="9" width="7.77734375" style="14" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" style="19" customWidth="1"/>
+    <col min="11" max="11" width="7.77734375" style="14" customWidth="1"/>
+    <col min="12" max="12" width="7.77734375" style="19" customWidth="1"/>
+    <col min="13" max="13" width="7.77734375" style="14" customWidth="1"/>
+    <col min="14" max="14" width="7.77734375" style="19" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" style="14" customWidth="1"/>
+    <col min="16" max="16" width="7.77734375" style="19" customWidth="1"/>
+    <col min="17" max="17" width="1.77734375" style="14" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" s="5" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:17" s="5" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -2755,83 +2783,76 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="2:17" s="7" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:17" s="7" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6"/>
-      <c r="C2" s="24" t="str">
-        <f ca="1">TEXT(C3,"aaa")</f>
+      <c r="C2" s="22" t="str">
+        <f>TEXT(C3,"aaa")</f>
         <v>日</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="28" t="str">
-        <f ca="1">TEXT(E3,"aaa")</f>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24" t="str">
+        <f>TEXT(E3,"aaa")</f>
         <v>一</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="29" t="str">
-        <f ca="1">TEXT(G3,"aaa")</f>
+      <c r="F2" s="23"/>
+      <c r="G2" s="25" t="str">
+        <f>TEXT(G3,"aaa")</f>
         <v>二</v>
       </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="28" t="str">
-        <f ca="1">TEXT(I3,"aaa")</f>
+      <c r="H2" s="25"/>
+      <c r="I2" s="24" t="str">
+        <f>TEXT(I3,"aaa")</f>
         <v>三</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="29" t="str">
-        <f ca="1">TEXT(K3,"aaa")</f>
+      <c r="J2" s="23"/>
+      <c r="K2" s="25" t="str">
+        <f>TEXT(K3,"aaa")</f>
         <v>四</v>
       </c>
-      <c r="L2" s="29"/>
-      <c r="M2" s="28" t="str">
-        <f ca="1">TEXT(M3,"aaa")</f>
+      <c r="L2" s="25"/>
+      <c r="M2" s="24" t="str">
+        <f>TEXT(M3,"aaa")</f>
         <v>五</v>
       </c>
-      <c r="N2" s="25"/>
-      <c r="O2" s="28" t="str">
-        <f ca="1">TEXT(O3,"aaa")</f>
+      <c r="N2" s="23"/>
+      <c r="O2" s="24" t="str">
+        <f>TEXT(O3,"aaa")</f>
         <v>六</v>
       </c>
-      <c r="P2" s="29"/>
+      <c r="P2" s="25"/>
     </row>
-    <row r="3" spans="2:17" s="7" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:17" s="7" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
-      <c r="C3" s="22">
-        <f ca="1">TODAY()-WEEKDAY(TODAY(),1)+1</f>
-        <v>44913</v>
-      </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="26">
-        <f ca="1">First_Day+1</f>
-        <v>44914</v>
-      </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="27">
-        <f ca="1">First_Day+2</f>
-        <v>44915</v>
+      <c r="C3" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="27"/>
+      <c r="G3" s="28" t="s">
+        <v>26</v>
       </c>
       <c r="H3" s="27"/>
-      <c r="I3" s="26">
-        <f ca="1">First_Day+3</f>
-        <v>44916</v>
-      </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="27">
-        <f ca="1">First_Day+4</f>
-        <v>44917</v>
+      <c r="I3" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="27"/>
+      <c r="K3" s="28" t="s">
+        <v>28</v>
       </c>
       <c r="L3" s="27"/>
-      <c r="M3" s="26">
-        <f ca="1">First_Day+5</f>
-        <v>44918</v>
-      </c>
-      <c r="N3" s="23"/>
-      <c r="O3" s="26">
-        <f ca="1">First_Day+6</f>
-        <v>44919</v>
-      </c>
-      <c r="P3" s="27"/>
+      <c r="M3" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="27"/>
+      <c r="O3" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="29"/>
     </row>
-    <row r="4" spans="2:17" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:17" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
@@ -2878,7 +2899,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:17" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:17" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
         <v>1</v>
       </c>
@@ -2901,7 +2922,7 @@
       <c r="O5" s="16"/>
       <c r="P5" s="20"/>
     </row>
-    <row r="6" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="15" t="s">
         <v>2</v>
       </c>
@@ -2924,7 +2945,7 @@
       <c r="O6" s="16"/>
       <c r="P6" s="20"/>
     </row>
-    <row r="7" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
@@ -2945,7 +2966,7 @@
       <c r="O7" s="16"/>
       <c r="P7" s="20"/>
     </row>
-    <row r="8" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
         <v>4</v>
       </c>
@@ -2964,7 +2985,7 @@
       <c r="O8" s="16"/>
       <c r="P8" s="20"/>
     </row>
-    <row r="9" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
         <v>5</v>
       </c>
@@ -2983,7 +3004,7 @@
       <c r="O9" s="16"/>
       <c r="P9" s="20"/>
     </row>
-    <row r="10" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
         <v>6</v>
       </c>
@@ -3002,7 +3023,7 @@
       <c r="O10" s="16"/>
       <c r="P10" s="20"/>
     </row>
-    <row r="11" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
         <v>7</v>
       </c>
@@ -3021,7 +3042,7 @@
       <c r="O11" s="16"/>
       <c r="P11" s="20"/>
     </row>
-    <row r="12" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
         <v>8</v>
       </c>
@@ -3040,7 +3061,7 @@
       <c r="O12" s="16"/>
       <c r="P12" s="20"/>
     </row>
-    <row r="13" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
         <v>9</v>
       </c>
@@ -3059,7 +3080,7 @@
       <c r="O13" s="16"/>
       <c r="P13" s="20"/>
     </row>
-    <row r="14" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
         <v>10</v>
       </c>
@@ -3078,7 +3099,7 @@
       <c r="O14" s="16"/>
       <c r="P14" s="20"/>
     </row>
-    <row r="15" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
         <v>11</v>
       </c>
@@ -3097,7 +3118,7 @@
       <c r="O15" s="16"/>
       <c r="P15" s="20"/>
     </row>
-    <row r="16" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
         <v>12</v>
       </c>
@@ -3116,7 +3137,7 @@
       <c r="O16" s="16"/>
       <c r="P16" s="20"/>
     </row>
-    <row r="17" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
         <v>13</v>
       </c>
@@ -3135,7 +3156,7 @@
       <c r="O17" s="16"/>
       <c r="P17" s="20"/>
     </row>
-    <row r="18" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
         <v>14</v>
       </c>
@@ -3154,7 +3175,7 @@
       <c r="O18" s="16"/>
       <c r="P18" s="20"/>
     </row>
-    <row r="19" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="s">
         <v>15</v>
       </c>
@@ -3173,7 +3194,7 @@
       <c r="O19" s="16"/>
       <c r="P19" s="20"/>
     </row>
-    <row r="20" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="15" t="s">
         <v>16</v>
       </c>
@@ -3192,7 +3213,7 @@
       <c r="O20" s="16"/>
       <c r="P20" s="20"/>
     </row>
-    <row r="21" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="15" t="s">
         <v>17</v>
       </c>
@@ -3231,7 +3252,7 @@
   <phoneticPr fontId="25" type="noConversion"/>
   <dataValidations xWindow="283" yWindow="632" count="11">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="每周家务安排表" prompt="_x000a_在单元格 C3 中输入开始日期。表中的每一天都有一个“人员”列，用于为每项家务分配人员。在“已完成”列下双击单元格即可轻松将各项任务标记为完成。" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="输入家务安排表当周的第 1 日。" sqref="C3" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="输入家务安排表当周的第 1 日。" sqref="C3" xr:uid="{329110E5-8C1D-4FDE-A182-3BB4C4C0581B}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="在此列中，输入为第 1 日各项家务分配的人员的姓名。" sqref="C4" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="在此列中，输入为第 2 日各项家务分配的人员的姓名。" sqref="E4" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="在此列中，输入为第 3 日各项家务分配的人员的姓名。" sqref="G4" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
@@ -3278,24 +3299,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3b47856d4cf355c0dacb39e1084d14f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a845a615265fdb1f7b12cc65ac20ecbd" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3503,25 +3506,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E60A8B6F-A245-4A02-AD66-F6A27855DC90}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61D8B24C-3B85-4379-80DC-A0BB54E539A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA919527-0680-40C7-8319-A14A2B99BD22}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3539,4 +3542,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61D8B24C-3B85-4379-80DC-A0BB54E539A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E60A8B6F-A245-4A02-AD66-F6A27855DC90}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>